<commit_message>
receding working with battery but with many problems
</commit_message>
<xml_diff>
--- a/output/teste/df_split0.xlsx
+++ b/output/teste/df_split0.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -614,251 +614,6 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>95.10188558031456</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>142.6528283704718</v>
-      </c>
-      <c r="H7">
-        <v>0.34</v>
-      </c>
-      <c r="I7">
-        <v>0.5</v>
-      </c>
-      <c r="J7">
-        <v>0.11</v>
-      </c>
-      <c r="K7">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>100.6937895111742</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>151.0406842667613</v>
-      </c>
-      <c r="H8">
-        <v>0.39</v>
-      </c>
-      <c r="I8">
-        <v>0.45</v>
-      </c>
-      <c r="J8">
-        <v>0.14</v>
-      </c>
-      <c r="K8">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>122.9626083453766</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>184.4439125180649</v>
-      </c>
-      <c r="H9">
-        <v>0.4</v>
-      </c>
-      <c r="I9">
-        <v>0.44</v>
-      </c>
-      <c r="J9">
-        <v>0.19</v>
-      </c>
-      <c r="K9">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>217.7285845022828</v>
-      </c>
-      <c r="D10">
-        <v>0.00555556</v>
-      </c>
-      <c r="E10">
-        <v>0.00555556</v>
-      </c>
-      <c r="F10">
-        <v>0.01111112</v>
-      </c>
-      <c r="G10">
-        <v>326.5928767534242</v>
-      </c>
-      <c r="H10">
-        <v>0.38</v>
-      </c>
-      <c r="I10">
-        <v>0.41</v>
-      </c>
-      <c r="J10">
-        <v>0.17</v>
-      </c>
-      <c r="K10">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>340.6121553362682</v>
-      </c>
-      <c r="D11">
-        <v>0.02222224</v>
-      </c>
-      <c r="E11">
-        <v>0.02222224</v>
-      </c>
-      <c r="F11">
-        <v>0.04444448</v>
-      </c>
-      <c r="G11">
-        <v>510.9182330044023</v>
-      </c>
-      <c r="H11">
-        <v>0.38</v>
-      </c>
-      <c r="I11">
-        <v>0.47</v>
-      </c>
-      <c r="J11">
-        <v>0.18</v>
-      </c>
-      <c r="K11">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12">
-        <v>428.3635523572899</v>
-      </c>
-      <c r="D12">
-        <v>0.08611118000000001</v>
-      </c>
-      <c r="E12">
-        <v>0.08611118000000001</v>
-      </c>
-      <c r="F12">
-        <v>0.17222236</v>
-      </c>
-      <c r="G12">
-        <v>642.5453285359349</v>
-      </c>
-      <c r="H12">
-        <v>0.4</v>
-      </c>
-      <c r="I12">
-        <v>0.45</v>
-      </c>
-      <c r="J12">
-        <v>0.12</v>
-      </c>
-      <c r="K12">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13">
-        <v>498.7069374946091</v>
-      </c>
-      <c r="D13">
-        <v>0.10000008</v>
-      </c>
-      <c r="E13">
-        <v>0.10000008</v>
-      </c>
-      <c r="F13">
-        <v>0.20000016</v>
-      </c>
-      <c r="G13">
-        <v>748.0604062419137</v>
-      </c>
-      <c r="H13">
-        <v>0.34</v>
-      </c>
-      <c r="I13">
-        <v>0.42</v>
-      </c>
-      <c r="J13">
-        <v>0.14</v>
-      </c>
-      <c r="K13">
-        <v>0.3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>